<commit_message>
update install variable design
</commit_message>
<xml_diff>
--- a/homecredit/vardesign/var_installments_payments.xlsx
+++ b/homecredit/vardesign/var_installments_payments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="117">
   <si>
     <t>Table</t>
   </si>
@@ -298,15 +298,9 @@
     <t>exobj</t>
   </si>
   <si>
-    <t>SK_DPD</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>CAC</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -326,6 +320,66 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>贷款数</t>
+  </si>
+  <si>
+    <t>SIP</t>
+  </si>
+  <si>
+    <t>SK_ID_PREV + '_''+DAYS_INSTALMENT</t>
+  </si>
+  <si>
+    <t>ID_PREV_NINS</t>
+  </si>
+  <si>
+    <t>IPN</t>
+  </si>
+  <si>
+    <t>DAYS_INSTALMENT_B</t>
+  </si>
+  <si>
+    <t>DAYS_ENTRY_PAYMENT_B</t>
+  </si>
+  <si>
+    <t>DAYS_ENTRY_PAYMENT_E</t>
+  </si>
+  <si>
+    <t>DAYS_ENTRY_PAYMENT_L</t>
+  </si>
+  <si>
+    <t>最早的还款日期</t>
+  </si>
+  <si>
+    <t>最晚的还款日期</t>
+  </si>
+  <si>
+    <t>min(DAYS_ENTRY_PAYMENT)</t>
+  </si>
+  <si>
+    <t>max(DAYS_ENTRY_PAYMENT)</t>
+  </si>
+  <si>
+    <t>step2. var_b2</t>
+  </si>
+  <si>
+    <t>DEE</t>
+  </si>
+  <si>
+    <t>DIFF_DAYS_ENTRY_EL</t>
+  </si>
+  <si>
+    <t>DDP</t>
+  </si>
+  <si>
+    <t>DAYS_ENTRY_PAYMENT_L - DAYS_ENTRY_PAYMENT_E</t>
+  </si>
+  <si>
+    <t>insrvrpb2</t>
+  </si>
+  <si>
+    <t>install of revolving repay batch 2</t>
   </si>
 </sst>
 </file>
@@ -816,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,7 +884,8 @@
     <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.25">
@@ -961,7 +1016,7 @@
         <v>14</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -983,7 +1038,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>103</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1035,19 +1090,17 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="I16" s="2" t="s">
-        <v>89</v>
+      <c r="I16" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1062,8 +1115,17 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
@@ -1078,8 +1140,17 @@
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
@@ -1094,8 +1165,17 @@
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
@@ -1110,8 +1190,17 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1126,8 +1215,17 @@
       <c r="G21" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1142,8 +1240,19 @@
       <c r="G22" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
@@ -1158,8 +1267,19 @@
       <c r="G23" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1175,7 +1295,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1311,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1209,103 +1329,604 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E27" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="E28" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>38</v>
+      <c r="C29" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="I49" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I50" t="s">
+        <v>115</v>
+      </c>
+      <c r="J50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="I52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M54" s="2"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="M55" s="2"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M56" s="2"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B61" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B62" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B63" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B64" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>